<commit_message>
Add multiple-choice question design function
</commit_message>
<xml_diff>
--- a/card/card_template.xlsx
+++ b/card/card_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\wenjian\anaconda3_project\li-scanner\card\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0CF5CBB1-09F6-4FA6-8ABD-6E516EBE37E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D12EEA40-39B4-4ABB-B3F9-07CC20DF91F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5304" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{1D6B9B70-82FD-4463-87AC-6908223E7A96}"/>
+    <workbookView xWindow="6444" yWindow="1224" windowWidth="13476" windowHeight="10056" xr2:uid="{04FE8028-6395-4A01-A937-3DD3844B3CF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="42">
   <si>
     <t>█</t>
   </si>
@@ -47,7 +47,7 @@
     <t>▍</t>
   </si>
   <si>
-    <t>数学答题卡</t>
+    <t>英语答题卡</t>
   </si>
   <si>
     <t>班
@@ -112,7 +112,7 @@
     <t>考试需知</t>
   </si>
   <si>
-    <t>考试加油</t>
+    <t>加油</t>
   </si>
   <si>
     <t>[ A ]</t>
@@ -131,6 +131,15 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>[ E ]</t>
+  </si>
+  <si>
+    <t>[ F ]</t>
+  </si>
+  <si>
+    <t>[ G ]</t>
+  </si>
+  <si>
     <t>填空题</t>
   </si>
   <si>
@@ -138,6 +147,12 @@
   </si>
   <si>
     <t>大题</t>
+  </si>
+  <si>
+    <t>47(1)</t>
+  </si>
+  <si>
+    <t>47(2)</t>
   </si>
   <si>
     <t>48(1)</t>
@@ -956,10 +971,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{974716B0-7AEB-4927-B659-0E2351612797}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEFDC444-F9F0-4B7C-BE09-D5487984569F}">
   <dimension ref="A1:Z124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1063,6 +1078,12 @@
       <c r="V2" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="W2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
     </row>
@@ -1514,9 +1535,7 @@
       <c r="F16" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="45" t="s">
-        <v>26</v>
-      </c>
+      <c r="G16" s="45"/>
       <c r="H16" s="45">
         <v>6</v>
       </c>
@@ -1581,9 +1600,7 @@
       <c r="F17" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="45" t="s">
-        <v>26</v>
-      </c>
+      <c r="G17" s="45"/>
       <c r="H17" s="45">
         <v>7</v>
       </c>
@@ -1648,9 +1665,7 @@
       <c r="F18" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="45" t="s">
-        <v>26</v>
-      </c>
+      <c r="G18" s="45"/>
       <c r="H18" s="45">
         <v>8</v>
       </c>
@@ -1906,21 +1921,11 @@
       <c r="Q22" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="R22" s="45">
-        <v>36</v>
-      </c>
-      <c r="S22" s="45" t="s">
-        <v>23</v>
-      </c>
-      <c r="T22" s="45" t="s">
-        <v>24</v>
-      </c>
-      <c r="U22" s="45" t="s">
-        <v>25</v>
-      </c>
-      <c r="V22" s="45" t="s">
-        <v>26</v>
-      </c>
+      <c r="R22" s="45"/>
+      <c r="S22" s="45"/>
+      <c r="T22" s="45"/>
+      <c r="U22" s="45"/>
+      <c r="V22" s="45"/>
       <c r="W22" s="45"/>
       <c r="X22" s="45"/>
     </row>
@@ -1973,21 +1978,11 @@
       <c r="Q23" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="R23" s="45">
-        <v>37</v>
-      </c>
-      <c r="S23" s="45" t="s">
-        <v>23</v>
-      </c>
-      <c r="T23" s="45" t="s">
-        <v>24</v>
-      </c>
-      <c r="U23" s="45" t="s">
-        <v>25</v>
-      </c>
-      <c r="V23" s="45" t="s">
-        <v>26</v>
-      </c>
+      <c r="R23" s="45"/>
+      <c r="S23" s="45"/>
+      <c r="T23" s="45"/>
+      <c r="U23" s="45"/>
+      <c r="V23" s="45"/>
       <c r="W23" s="45"/>
       <c r="X23" s="45"/>
     </row>
@@ -2040,21 +2035,11 @@
       <c r="Q24" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="R24" s="45">
-        <v>38</v>
-      </c>
-      <c r="S24" s="45" t="s">
-        <v>23</v>
-      </c>
-      <c r="T24" s="45" t="s">
-        <v>24</v>
-      </c>
-      <c r="U24" s="45" t="s">
-        <v>25</v>
-      </c>
-      <c r="V24" s="45" t="s">
-        <v>26</v>
-      </c>
+      <c r="R24" s="45"/>
+      <c r="S24" s="45"/>
+      <c r="T24" s="45"/>
+      <c r="U24" s="45"/>
+      <c r="V24" s="45"/>
       <c r="W24" s="45"/>
       <c r="X24" s="45"/>
     </row>
@@ -2107,21 +2092,11 @@
       <c r="Q25" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="R25" s="45">
-        <v>39</v>
-      </c>
-      <c r="S25" s="45" t="s">
-        <v>23</v>
-      </c>
-      <c r="T25" s="45" t="s">
-        <v>24</v>
-      </c>
-      <c r="U25" s="45" t="s">
-        <v>25</v>
-      </c>
-      <c r="V25" s="45" t="s">
-        <v>26</v>
-      </c>
+      <c r="R25" s="45"/>
+      <c r="S25" s="45"/>
+      <c r="T25" s="45"/>
+      <c r="U25" s="45"/>
+      <c r="V25" s="45"/>
       <c r="W25" s="45"/>
       <c r="X25" s="45"/>
     </row>
@@ -2174,21 +2149,11 @@
       <c r="Q26" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="R26" s="45">
-        <v>40</v>
-      </c>
-      <c r="S26" s="45" t="s">
-        <v>23</v>
-      </c>
-      <c r="T26" s="45" t="s">
-        <v>24</v>
-      </c>
-      <c r="U26" s="45" t="s">
-        <v>25</v>
-      </c>
-      <c r="V26" s="45" t="s">
-        <v>26</v>
-      </c>
+      <c r="R26" s="45"/>
+      <c r="S26" s="45"/>
+      <c r="T26" s="45"/>
+      <c r="U26" s="45"/>
+      <c r="V26" s="45"/>
       <c r="W26" s="45"/>
       <c r="X26" s="45"/>
     </row>
@@ -2217,161 +2182,250 @@
       <c r="X27" s="45"/>
     </row>
     <row r="28" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="C28" s="45"/>
-      <c r="D28" s="50" t="s">
+      <c r="B28" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="45">
+        <v>36</v>
+      </c>
+      <c r="D28" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="G28" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="H28" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="51"/>
-      <c r="F28" s="52"/>
-      <c r="G28" s="52"/>
-      <c r="H28" s="52"/>
-      <c r="I28" s="52"/>
-      <c r="J28" s="52"/>
-      <c r="K28" s="52"/>
-      <c r="L28" s="52"/>
-      <c r="M28" s="52"/>
-      <c r="N28" s="52"/>
-      <c r="O28" s="52"/>
-      <c r="P28" s="52"/>
-      <c r="Q28" s="52"/>
-      <c r="R28" s="52"/>
-      <c r="S28" s="52"/>
-      <c r="T28" s="52"/>
-      <c r="U28" s="52"/>
-      <c r="V28" s="52"/>
-      <c r="W28" s="55"/>
+      <c r="I28" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="J28" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="K28" s="45"/>
+      <c r="L28" s="45"/>
+      <c r="M28" s="45"/>
+      <c r="N28" s="45"/>
+      <c r="O28" s="45"/>
+      <c r="P28" s="45"/>
+      <c r="Q28" s="45"/>
+      <c r="R28" s="45"/>
+      <c r="S28" s="45"/>
+      <c r="T28" s="45"/>
+      <c r="U28" s="45"/>
+      <c r="V28" s="45"/>
+      <c r="W28" s="45"/>
       <c r="X28" s="45"/>
     </row>
     <row r="29" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="C29" s="45"/>
-      <c r="D29" s="49"/>
-      <c r="E29" s="48"/>
-      <c r="F29" s="48"/>
-      <c r="G29" s="48"/>
-      <c r="H29" s="48"/>
-      <c r="I29" s="48"/>
-      <c r="J29" s="48"/>
-      <c r="K29" s="48"/>
-      <c r="L29" s="48"/>
-      <c r="M29" s="48"/>
-      <c r="N29" s="48"/>
-      <c r="O29" s="48"/>
-      <c r="P29" s="48"/>
-      <c r="Q29" s="48"/>
-      <c r="R29" s="48"/>
-      <c r="S29" s="48"/>
-      <c r="T29" s="48"/>
-      <c r="U29" s="48"/>
-      <c r="V29" s="48"/>
-      <c r="W29" s="56"/>
+      <c r="B29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="45">
+        <v>37</v>
+      </c>
+      <c r="D29" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="F29" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="G29" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="H29" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="I29" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="J29" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="K29" s="45"/>
+      <c r="L29" s="45"/>
+      <c r="M29" s="45"/>
+      <c r="N29" s="45"/>
+      <c r="O29" s="45"/>
+      <c r="P29" s="45"/>
+      <c r="Q29" s="45"/>
+      <c r="R29" s="45"/>
+      <c r="S29" s="45"/>
+      <c r="T29" s="45"/>
+      <c r="U29" s="45"/>
+      <c r="V29" s="45"/>
+      <c r="W29" s="45"/>
       <c r="X29" s="45"/>
     </row>
     <row r="30" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="C30" s="45"/>
-      <c r="D30" s="46" t="s">
+      <c r="B30" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="45">
+        <v>38</v>
+      </c>
+      <c r="D30" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="E30" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="F30" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="G30" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="H30" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="I30" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
-      <c r="K30" s="47"/>
-      <c r="L30" s="47"/>
-      <c r="M30" s="47"/>
-      <c r="N30" s="47"/>
-      <c r="O30" s="47"/>
-      <c r="P30" s="47"/>
-      <c r="Q30" s="47"/>
-      <c r="R30" s="47"/>
-      <c r="S30" s="47"/>
-      <c r="T30" s="47"/>
-      <c r="U30" s="47"/>
-      <c r="V30" s="47"/>
-      <c r="W30" s="70"/>
+      <c r="J30" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="K30" s="45"/>
+      <c r="L30" s="45"/>
+      <c r="M30" s="45"/>
+      <c r="N30" s="45"/>
+      <c r="O30" s="45"/>
+      <c r="P30" s="45"/>
+      <c r="Q30" s="45"/>
+      <c r="R30" s="45"/>
+      <c r="S30" s="45"/>
+      <c r="T30" s="45"/>
+      <c r="U30" s="45"/>
+      <c r="V30" s="45"/>
+      <c r="W30" s="45"/>
       <c r="X30" s="45"/>
     </row>
     <row r="31" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="C31" s="45"/>
-      <c r="D31" s="49"/>
-      <c r="E31" s="48"/>
-      <c r="F31" s="48"/>
-      <c r="G31" s="48"/>
-      <c r="H31" s="48"/>
-      <c r="I31" s="48"/>
-      <c r="J31" s="48"/>
-      <c r="K31" s="48"/>
-      <c r="L31" s="48"/>
-      <c r="M31" s="48"/>
-      <c r="N31" s="48"/>
-      <c r="O31" s="48"/>
-      <c r="P31" s="48"/>
-      <c r="Q31" s="48"/>
-      <c r="R31" s="48"/>
-      <c r="S31" s="48"/>
-      <c r="T31" s="48"/>
-      <c r="U31" s="48"/>
-      <c r="V31" s="48"/>
-      <c r="W31" s="56"/>
+      <c r="B31" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="45">
+        <v>39</v>
+      </c>
+      <c r="D31" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="G31" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="H31" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="I31" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="J31" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="K31" s="45"/>
+      <c r="L31" s="45"/>
+      <c r="M31" s="45"/>
+      <c r="N31" s="45"/>
+      <c r="O31" s="45"/>
+      <c r="P31" s="45"/>
+      <c r="Q31" s="45"/>
+      <c r="R31" s="45"/>
+      <c r="S31" s="45"/>
+      <c r="T31" s="45"/>
+      <c r="U31" s="45"/>
+      <c r="V31" s="45"/>
+      <c r="W31" s="45"/>
       <c r="X31" s="45"/>
     </row>
     <row r="32" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="C32" s="45"/>
-      <c r="D32" s="67"/>
-      <c r="E32" s="68"/>
-      <c r="F32" s="68"/>
-      <c r="G32" s="68"/>
-      <c r="H32" s="68"/>
-      <c r="I32" s="68"/>
-      <c r="J32" s="68"/>
-      <c r="K32" s="68"/>
-      <c r="L32" s="68"/>
-      <c r="M32" s="68"/>
-      <c r="N32" s="68"/>
-      <c r="O32" s="68"/>
-      <c r="P32" s="68"/>
-      <c r="Q32" s="68"/>
-      <c r="R32" s="68"/>
-      <c r="S32" s="68"/>
-      <c r="T32" s="68"/>
-      <c r="U32" s="68"/>
-      <c r="V32" s="68"/>
-      <c r="W32" s="69"/>
+      <c r="B32" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="45">
+        <v>40</v>
+      </c>
+      <c r="D32" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="F32" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="G32" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="H32" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="I32" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="J32" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="K32" s="45"/>
+      <c r="L32" s="45"/>
+      <c r="M32" s="45"/>
+      <c r="N32" s="45"/>
+      <c r="O32" s="45"/>
+      <c r="P32" s="45"/>
+      <c r="Q32" s="45"/>
+      <c r="R32" s="45"/>
+      <c r="S32" s="45"/>
+      <c r="T32" s="45"/>
+      <c r="U32" s="45"/>
+      <c r="V32" s="45"/>
+      <c r="W32" s="45"/>
       <c r="X32" s="45"/>
     </row>
     <row r="33" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C33" s="45"/>
-      <c r="D33" s="46" t="s">
-        <v>30</v>
-      </c>
-      <c r="E33" s="47"/>
-      <c r="F33" s="48"/>
-      <c r="G33" s="48"/>
-      <c r="H33" s="48"/>
-      <c r="I33" s="48"/>
-      <c r="J33" s="48"/>
-      <c r="K33" s="48"/>
-      <c r="L33" s="48"/>
-      <c r="M33" s="48"/>
-      <c r="N33" s="48"/>
-      <c r="O33" s="48"/>
-      <c r="P33" s="48"/>
-      <c r="Q33" s="48"/>
-      <c r="R33" s="48"/>
-      <c r="S33" s="48"/>
-      <c r="T33" s="48"/>
-      <c r="U33" s="48"/>
-      <c r="V33" s="48"/>
-      <c r="W33" s="56"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="45"/>
+      <c r="H33" s="45"/>
+      <c r="I33" s="45"/>
+      <c r="J33" s="45"/>
+      <c r="K33" s="45"/>
+      <c r="L33" s="45"/>
+      <c r="M33" s="45"/>
+      <c r="N33" s="45"/>
+      <c r="O33" s="45"/>
+      <c r="P33" s="45"/>
+      <c r="Q33" s="45"/>
+      <c r="R33" s="45"/>
+      <c r="S33" s="45"/>
+      <c r="T33" s="45"/>
+      <c r="U33" s="45"/>
+      <c r="V33" s="45"/>
+      <c r="W33" s="45"/>
       <c r="X33" s="45"/>
     </row>
     <row r="34" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C34" s="45"/>
-      <c r="D34" s="71">
-        <v>46</v>
-      </c>
-      <c r="E34" s="52"/>
+      <c r="D34" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="E34" s="51"/>
       <c r="F34" s="52"/>
       <c r="G34" s="52"/>
       <c r="H34" s="52"/>
@@ -2418,26 +2472,28 @@
     </row>
     <row r="36" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C36" s="45"/>
-      <c r="D36" s="49"/>
-      <c r="E36" s="48"/>
-      <c r="F36" s="48"/>
-      <c r="G36" s="48"/>
-      <c r="H36" s="48"/>
-      <c r="I36" s="48"/>
-      <c r="J36" s="48"/>
-      <c r="K36" s="48"/>
-      <c r="L36" s="48"/>
-      <c r="M36" s="48"/>
-      <c r="N36" s="48"/>
-      <c r="O36" s="48"/>
-      <c r="P36" s="48"/>
-      <c r="Q36" s="48"/>
-      <c r="R36" s="48"/>
-      <c r="S36" s="48"/>
-      <c r="T36" s="48"/>
-      <c r="U36" s="48"/>
-      <c r="V36" s="48"/>
-      <c r="W36" s="56"/>
+      <c r="D36" s="46" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" s="47"/>
+      <c r="F36" s="47"/>
+      <c r="G36" s="47"/>
+      <c r="H36" s="47"/>
+      <c r="I36" s="47"/>
+      <c r="J36" s="47"/>
+      <c r="K36" s="47"/>
+      <c r="L36" s="47"/>
+      <c r="M36" s="47"/>
+      <c r="N36" s="47"/>
+      <c r="O36" s="47"/>
+      <c r="P36" s="47"/>
+      <c r="Q36" s="47"/>
+      <c r="R36" s="47"/>
+      <c r="S36" s="47"/>
+      <c r="T36" s="47"/>
+      <c r="U36" s="47"/>
+      <c r="V36" s="47"/>
+      <c r="W36" s="70"/>
       <c r="X36" s="45"/>
     </row>
     <row r="37" spans="3:24" x14ac:dyDescent="0.25">
@@ -2466,32 +2522,34 @@
     </row>
     <row r="38" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C38" s="45"/>
-      <c r="D38" s="49"/>
-      <c r="E38" s="48"/>
-      <c r="F38" s="48"/>
-      <c r="G38" s="48"/>
-      <c r="H38" s="48"/>
-      <c r="I38" s="48"/>
-      <c r="J38" s="48"/>
-      <c r="K38" s="48"/>
-      <c r="L38" s="48"/>
-      <c r="M38" s="48"/>
-      <c r="N38" s="48"/>
-      <c r="O38" s="48"/>
-      <c r="P38" s="48"/>
-      <c r="Q38" s="48"/>
-      <c r="R38" s="48"/>
-      <c r="S38" s="48"/>
-      <c r="T38" s="48"/>
-      <c r="U38" s="48"/>
-      <c r="V38" s="48"/>
-      <c r="W38" s="56"/>
+      <c r="D38" s="67"/>
+      <c r="E38" s="68"/>
+      <c r="F38" s="68"/>
+      <c r="G38" s="68"/>
+      <c r="H38" s="68"/>
+      <c r="I38" s="68"/>
+      <c r="J38" s="68"/>
+      <c r="K38" s="68"/>
+      <c r="L38" s="68"/>
+      <c r="M38" s="68"/>
+      <c r="N38" s="68"/>
+      <c r="O38" s="68"/>
+      <c r="P38" s="68"/>
+      <c r="Q38" s="68"/>
+      <c r="R38" s="68"/>
+      <c r="S38" s="68"/>
+      <c r="T38" s="68"/>
+      <c r="U38" s="68"/>
+      <c r="V38" s="68"/>
+      <c r="W38" s="69"/>
       <c r="X38" s="45"/>
     </row>
     <row r="39" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C39" s="45"/>
-      <c r="D39" s="49"/>
-      <c r="E39" s="48"/>
+      <c r="D39" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="E39" s="47"/>
       <c r="F39" s="48"/>
       <c r="G39" s="48"/>
       <c r="H39" s="48"/>
@@ -2515,7 +2573,7 @@
     <row r="40" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C40" s="45"/>
       <c r="D40" s="71">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E40" s="52"/>
       <c r="F40" s="52"/>
@@ -2661,7 +2719,7 @@
     <row r="46" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C46" s="45"/>
       <c r="D46" s="71" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E46" s="52"/>
       <c r="F46" s="52"/>
@@ -2807,7 +2865,7 @@
     <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C52" s="45"/>
       <c r="D52" s="71" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E52" s="52"/>
       <c r="F52" s="52"/>
@@ -3056,7 +3114,7 @@
     </row>
     <row r="66" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D66" s="58" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E66" s="59"/>
       <c r="F66" s="59"/>
@@ -3190,7 +3248,7 @@
     </row>
     <row r="72" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D72" s="58" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E72" s="59"/>
       <c r="F72" s="59"/>
@@ -3324,7 +3382,7 @@
     </row>
     <row r="78" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D78" s="58" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E78" s="59"/>
       <c r="F78" s="59"/>
@@ -3458,7 +3516,7 @@
     </row>
     <row r="84" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D84" s="58" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E84" s="59"/>
       <c r="F84" s="59"/>
@@ -3591,26 +3649,28 @@
       <c r="W89" s="63"/>
     </row>
     <row r="90" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D90" s="61"/>
-      <c r="E90" s="62"/>
-      <c r="F90" s="62"/>
-      <c r="G90" s="62"/>
-      <c r="H90" s="62"/>
-      <c r="I90" s="62"/>
-      <c r="J90" s="62"/>
-      <c r="K90" s="62"/>
-      <c r="L90" s="62"/>
-      <c r="M90" s="62"/>
-      <c r="N90" s="62"/>
-      <c r="O90" s="62"/>
-      <c r="P90" s="62"/>
-      <c r="Q90" s="62"/>
-      <c r="R90" s="62"/>
-      <c r="S90" s="62"/>
-      <c r="T90" s="62"/>
-      <c r="U90" s="62"/>
-      <c r="V90" s="62"/>
-      <c r="W90" s="63"/>
+      <c r="D90" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="E90" s="59"/>
+      <c r="F90" s="59"/>
+      <c r="G90" s="59"/>
+      <c r="H90" s="59"/>
+      <c r="I90" s="59"/>
+      <c r="J90" s="59"/>
+      <c r="K90" s="59"/>
+      <c r="L90" s="59"/>
+      <c r="M90" s="59"/>
+      <c r="N90" s="59"/>
+      <c r="O90" s="59"/>
+      <c r="P90" s="59"/>
+      <c r="Q90" s="59"/>
+      <c r="R90" s="59"/>
+      <c r="S90" s="59"/>
+      <c r="T90" s="59"/>
+      <c r="U90" s="59"/>
+      <c r="V90" s="59"/>
+      <c r="W90" s="60"/>
     </row>
     <row r="91" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D91" s="61"/>
@@ -3723,26 +3783,28 @@
       <c r="W95" s="63"/>
     </row>
     <row r="96" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D96" s="61"/>
-      <c r="E96" s="62"/>
-      <c r="F96" s="62"/>
-      <c r="G96" s="62"/>
-      <c r="H96" s="62"/>
-      <c r="I96" s="62"/>
-      <c r="J96" s="62"/>
-      <c r="K96" s="62"/>
-      <c r="L96" s="62"/>
-      <c r="M96" s="62"/>
-      <c r="N96" s="62"/>
-      <c r="O96" s="62"/>
-      <c r="P96" s="62"/>
-      <c r="Q96" s="62"/>
-      <c r="R96" s="62"/>
-      <c r="S96" s="62"/>
-      <c r="T96" s="62"/>
-      <c r="U96" s="62"/>
-      <c r="V96" s="62"/>
-      <c r="W96" s="63"/>
+      <c r="D96" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="E96" s="59"/>
+      <c r="F96" s="59"/>
+      <c r="G96" s="59"/>
+      <c r="H96" s="59"/>
+      <c r="I96" s="59"/>
+      <c r="J96" s="59"/>
+      <c r="K96" s="59"/>
+      <c r="L96" s="59"/>
+      <c r="M96" s="59"/>
+      <c r="N96" s="59"/>
+      <c r="O96" s="59"/>
+      <c r="P96" s="59"/>
+      <c r="Q96" s="59"/>
+      <c r="R96" s="59"/>
+      <c r="S96" s="59"/>
+      <c r="T96" s="59"/>
+      <c r="U96" s="59"/>
+      <c r="V96" s="59"/>
+      <c r="W96" s="60"/>
     </row>
     <row r="97" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D97" s="61"/>
@@ -4313,10 +4375,10 @@
   </sheetData>
   <mergeCells count="25">
     <mergeCell ref="R5:W14"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D30:W30"/>
-    <mergeCell ref="D32:W32"/>
-    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D36:W36"/>
+    <mergeCell ref="D38:W38"/>
+    <mergeCell ref="D39:E39"/>
     <mergeCell ref="A123:B124"/>
     <mergeCell ref="Y123:Z124"/>
     <mergeCell ref="C1:X1"/>

</xml_diff>

<commit_message>
Add answer recognition module
</commit_message>
<xml_diff>
--- a/card/card_template.xlsx
+++ b/card/card_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\wenjian\anaconda3_project\li-scanner\card\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D12EEA40-39B4-4ABB-B3F9-07CC20DF91F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{080E9947-F934-4966-9ED4-A761B1136DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6444" yWindow="1224" windowWidth="13476" windowHeight="10056" xr2:uid="{04FE8028-6395-4A01-A937-3DD3844B3CF3}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{8FD2E01E-F9BA-4223-AE66-67C1E8AA690D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="33">
   <si>
     <t>█</t>
   </si>
@@ -112,7 +112,7 @@
     <t>考试需知</t>
   </si>
   <si>
-    <t>加油</t>
+    <t>考试加油</t>
   </si>
   <si>
     <t>[ A ]</t>
@@ -143,34 +143,7 @@
     <t>填空题</t>
   </si>
   <si>
-    <t>41______________             42______________             43______________             44______________             45______________</t>
-  </si>
-  <si>
     <t>大题</t>
-  </si>
-  <si>
-    <t>47(1)</t>
-  </si>
-  <si>
-    <t>47(2)</t>
-  </si>
-  <si>
-    <t>48(1)</t>
-  </si>
-  <si>
-    <t>48(2)</t>
-  </si>
-  <si>
-    <t>49(1)</t>
-  </si>
-  <si>
-    <t>49(2)</t>
-  </si>
-  <si>
-    <t>50(1)</t>
-  </si>
-  <si>
-    <t>50(2)</t>
   </si>
 </sst>
 </file>
@@ -441,7 +414,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -650,12 +623,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -971,7 +938,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEFDC444-F9F0-4B7C-BE09-D5487984569F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B7A54DC-0357-409B-A8A5-E2923493BA82}">
   <dimension ref="A1:Z124"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1665,7 +1632,9 @@
       <c r="F18" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="45"/>
+      <c r="G18" s="45" t="s">
+        <v>26</v>
+      </c>
       <c r="H18" s="45">
         <v>8</v>
       </c>
@@ -2472,34 +2441,34 @@
     </row>
     <row r="36" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C36" s="45"/>
-      <c r="D36" s="46" t="s">
-        <v>32</v>
-      </c>
-      <c r="E36" s="47"/>
-      <c r="F36" s="47"/>
-      <c r="G36" s="47"/>
-      <c r="H36" s="47"/>
-      <c r="I36" s="47"/>
-      <c r="J36" s="47"/>
-      <c r="K36" s="47"/>
-      <c r="L36" s="47"/>
-      <c r="M36" s="47"/>
-      <c r="N36" s="47"/>
-      <c r="O36" s="47"/>
-      <c r="P36" s="47"/>
-      <c r="Q36" s="47"/>
-      <c r="R36" s="47"/>
-      <c r="S36" s="47"/>
-      <c r="T36" s="47"/>
-      <c r="U36" s="47"/>
-      <c r="V36" s="47"/>
-      <c r="W36" s="70"/>
+      <c r="D36" s="67"/>
+      <c r="E36" s="68"/>
+      <c r="F36" s="68"/>
+      <c r="G36" s="68"/>
+      <c r="H36" s="68"/>
+      <c r="I36" s="68"/>
+      <c r="J36" s="68"/>
+      <c r="K36" s="68"/>
+      <c r="L36" s="68"/>
+      <c r="M36" s="68"/>
+      <c r="N36" s="68"/>
+      <c r="O36" s="68"/>
+      <c r="P36" s="68"/>
+      <c r="Q36" s="68"/>
+      <c r="R36" s="68"/>
+      <c r="S36" s="68"/>
+      <c r="T36" s="68"/>
+      <c r="U36" s="68"/>
+      <c r="V36" s="68"/>
+      <c r="W36" s="69"/>
       <c r="X36" s="45"/>
     </row>
     <row r="37" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C37" s="45"/>
-      <c r="D37" s="49"/>
-      <c r="E37" s="48"/>
+      <c r="D37" s="46" t="s">
+        <v>32</v>
+      </c>
+      <c r="E37" s="47"/>
       <c r="F37" s="48"/>
       <c r="G37" s="48"/>
       <c r="H37" s="48"/>
@@ -2522,34 +2491,32 @@
     </row>
     <row r="38" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C38" s="45"/>
-      <c r="D38" s="67"/>
-      <c r="E38" s="68"/>
-      <c r="F38" s="68"/>
-      <c r="G38" s="68"/>
-      <c r="H38" s="68"/>
-      <c r="I38" s="68"/>
-      <c r="J38" s="68"/>
-      <c r="K38" s="68"/>
-      <c r="L38" s="68"/>
-      <c r="M38" s="68"/>
-      <c r="N38" s="68"/>
-      <c r="O38" s="68"/>
-      <c r="P38" s="68"/>
-      <c r="Q38" s="68"/>
-      <c r="R38" s="68"/>
-      <c r="S38" s="68"/>
-      <c r="T38" s="68"/>
-      <c r="U38" s="68"/>
-      <c r="V38" s="68"/>
-      <c r="W38" s="69"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="48"/>
+      <c r="F38" s="48"/>
+      <c r="G38" s="48"/>
+      <c r="H38" s="48"/>
+      <c r="I38" s="48"/>
+      <c r="J38" s="48"/>
+      <c r="K38" s="48"/>
+      <c r="L38" s="48"/>
+      <c r="M38" s="48"/>
+      <c r="N38" s="48"/>
+      <c r="O38" s="48"/>
+      <c r="P38" s="48"/>
+      <c r="Q38" s="48"/>
+      <c r="R38" s="48"/>
+      <c r="S38" s="48"/>
+      <c r="T38" s="48"/>
+      <c r="U38" s="48"/>
+      <c r="V38" s="48"/>
+      <c r="W38" s="56"/>
       <c r="X38" s="45"/>
     </row>
     <row r="39" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C39" s="45"/>
-      <c r="D39" s="46" t="s">
-        <v>33</v>
-      </c>
-      <c r="E39" s="47"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="48"/>
       <c r="F39" s="48"/>
       <c r="G39" s="48"/>
       <c r="H39" s="48"/>
@@ -2572,28 +2539,26 @@
     </row>
     <row r="40" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C40" s="45"/>
-      <c r="D40" s="71">
-        <v>46</v>
-      </c>
-      <c r="E40" s="52"/>
-      <c r="F40" s="52"/>
-      <c r="G40" s="52"/>
-      <c r="H40" s="52"/>
-      <c r="I40" s="52"/>
-      <c r="J40" s="52"/>
-      <c r="K40" s="52"/>
-      <c r="L40" s="52"/>
-      <c r="M40" s="52"/>
-      <c r="N40" s="52"/>
-      <c r="O40" s="52"/>
-      <c r="P40" s="52"/>
-      <c r="Q40" s="52"/>
-      <c r="R40" s="52"/>
-      <c r="S40" s="52"/>
-      <c r="T40" s="52"/>
-      <c r="U40" s="52"/>
-      <c r="V40" s="52"/>
-      <c r="W40" s="55"/>
+      <c r="D40" s="49"/>
+      <c r="E40" s="48"/>
+      <c r="F40" s="48"/>
+      <c r="G40" s="48"/>
+      <c r="H40" s="48"/>
+      <c r="I40" s="48"/>
+      <c r="J40" s="48"/>
+      <c r="K40" s="48"/>
+      <c r="L40" s="48"/>
+      <c r="M40" s="48"/>
+      <c r="N40" s="48"/>
+      <c r="O40" s="48"/>
+      <c r="P40" s="48"/>
+      <c r="Q40" s="48"/>
+      <c r="R40" s="48"/>
+      <c r="S40" s="48"/>
+      <c r="T40" s="48"/>
+      <c r="U40" s="48"/>
+      <c r="V40" s="48"/>
+      <c r="W40" s="56"/>
       <c r="X40" s="45"/>
     </row>
     <row r="41" spans="3:24" x14ac:dyDescent="0.25">
@@ -2718,28 +2683,26 @@
     </row>
     <row r="46" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C46" s="45"/>
-      <c r="D46" s="71" t="s">
-        <v>34</v>
-      </c>
-      <c r="E46" s="52"/>
-      <c r="F46" s="52"/>
-      <c r="G46" s="52"/>
-      <c r="H46" s="52"/>
-      <c r="I46" s="52"/>
-      <c r="J46" s="52"/>
-      <c r="K46" s="52"/>
-      <c r="L46" s="52"/>
-      <c r="M46" s="52"/>
-      <c r="N46" s="52"/>
-      <c r="O46" s="52"/>
-      <c r="P46" s="52"/>
-      <c r="Q46" s="52"/>
-      <c r="R46" s="52"/>
-      <c r="S46" s="52"/>
-      <c r="T46" s="52"/>
-      <c r="U46" s="52"/>
-      <c r="V46" s="52"/>
-      <c r="W46" s="55"/>
+      <c r="D46" s="49"/>
+      <c r="E46" s="48"/>
+      <c r="F46" s="48"/>
+      <c r="G46" s="48"/>
+      <c r="H46" s="48"/>
+      <c r="I46" s="48"/>
+      <c r="J46" s="48"/>
+      <c r="K46" s="48"/>
+      <c r="L46" s="48"/>
+      <c r="M46" s="48"/>
+      <c r="N46" s="48"/>
+      <c r="O46" s="48"/>
+      <c r="P46" s="48"/>
+      <c r="Q46" s="48"/>
+      <c r="R46" s="48"/>
+      <c r="S46" s="48"/>
+      <c r="T46" s="48"/>
+      <c r="U46" s="48"/>
+      <c r="V46" s="48"/>
+      <c r="W46" s="56"/>
       <c r="X46" s="45"/>
     </row>
     <row r="47" spans="3:24" x14ac:dyDescent="0.25">
@@ -2864,28 +2827,26 @@
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C52" s="45"/>
-      <c r="D52" s="71" t="s">
-        <v>35</v>
-      </c>
-      <c r="E52" s="52"/>
-      <c r="F52" s="52"/>
-      <c r="G52" s="52"/>
-      <c r="H52" s="52"/>
-      <c r="I52" s="52"/>
-      <c r="J52" s="52"/>
-      <c r="K52" s="52"/>
-      <c r="L52" s="52"/>
-      <c r="M52" s="52"/>
-      <c r="N52" s="52"/>
-      <c r="O52" s="52"/>
-      <c r="P52" s="52"/>
-      <c r="Q52" s="52"/>
-      <c r="R52" s="52"/>
-      <c r="S52" s="52"/>
-      <c r="T52" s="52"/>
-      <c r="U52" s="52"/>
-      <c r="V52" s="52"/>
-      <c r="W52" s="55"/>
+      <c r="D52" s="49"/>
+      <c r="E52" s="48"/>
+      <c r="F52" s="48"/>
+      <c r="G52" s="48"/>
+      <c r="H52" s="48"/>
+      <c r="I52" s="48"/>
+      <c r="J52" s="48"/>
+      <c r="K52" s="48"/>
+      <c r="L52" s="48"/>
+      <c r="M52" s="48"/>
+      <c r="N52" s="48"/>
+      <c r="O52" s="48"/>
+      <c r="P52" s="48"/>
+      <c r="Q52" s="48"/>
+      <c r="R52" s="48"/>
+      <c r="S52" s="48"/>
+      <c r="T52" s="48"/>
+      <c r="U52" s="48"/>
+      <c r="V52" s="48"/>
+      <c r="W52" s="56"/>
       <c r="X52" s="45"/>
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.25">
@@ -3113,9 +3074,7 @@
       <c r="Z64" s="2"/>
     </row>
     <row r="66" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D66" s="58" t="s">
-        <v>36</v>
-      </c>
+      <c r="D66" s="58"/>
       <c r="E66" s="59"/>
       <c r="F66" s="59"/>
       <c r="G66" s="59"/>
@@ -3247,28 +3206,26 @@
       <c r="W71" s="63"/>
     </row>
     <row r="72" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D72" s="58" t="s">
-        <v>37</v>
-      </c>
-      <c r="E72" s="59"/>
-      <c r="F72" s="59"/>
-      <c r="G72" s="59"/>
-      <c r="H72" s="59"/>
-      <c r="I72" s="59"/>
-      <c r="J72" s="59"/>
-      <c r="K72" s="59"/>
-      <c r="L72" s="59"/>
-      <c r="M72" s="59"/>
-      <c r="N72" s="59"/>
-      <c r="O72" s="59"/>
-      <c r="P72" s="59"/>
-      <c r="Q72" s="59"/>
-      <c r="R72" s="59"/>
-      <c r="S72" s="59"/>
-      <c r="T72" s="59"/>
-      <c r="U72" s="59"/>
-      <c r="V72" s="59"/>
-      <c r="W72" s="60"/>
+      <c r="D72" s="61"/>
+      <c r="E72" s="62"/>
+      <c r="F72" s="62"/>
+      <c r="G72" s="62"/>
+      <c r="H72" s="62"/>
+      <c r="I72" s="62"/>
+      <c r="J72" s="62"/>
+      <c r="K72" s="62"/>
+      <c r="L72" s="62"/>
+      <c r="M72" s="62"/>
+      <c r="N72" s="62"/>
+      <c r="O72" s="62"/>
+      <c r="P72" s="62"/>
+      <c r="Q72" s="62"/>
+      <c r="R72" s="62"/>
+      <c r="S72" s="62"/>
+      <c r="T72" s="62"/>
+      <c r="U72" s="62"/>
+      <c r="V72" s="62"/>
+      <c r="W72" s="63"/>
     </row>
     <row r="73" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D73" s="61"/>
@@ -3381,28 +3338,26 @@
       <c r="W77" s="63"/>
     </row>
     <row r="78" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D78" s="58" t="s">
-        <v>38</v>
-      </c>
-      <c r="E78" s="59"/>
-      <c r="F78" s="59"/>
-      <c r="G78" s="59"/>
-      <c r="H78" s="59"/>
-      <c r="I78" s="59"/>
-      <c r="J78" s="59"/>
-      <c r="K78" s="59"/>
-      <c r="L78" s="59"/>
-      <c r="M78" s="59"/>
-      <c r="N78" s="59"/>
-      <c r="O78" s="59"/>
-      <c r="P78" s="59"/>
-      <c r="Q78" s="59"/>
-      <c r="R78" s="59"/>
-      <c r="S78" s="59"/>
-      <c r="T78" s="59"/>
-      <c r="U78" s="59"/>
-      <c r="V78" s="59"/>
-      <c r="W78" s="60"/>
+      <c r="D78" s="61"/>
+      <c r="E78" s="62"/>
+      <c r="F78" s="62"/>
+      <c r="G78" s="62"/>
+      <c r="H78" s="62"/>
+      <c r="I78" s="62"/>
+      <c r="J78" s="62"/>
+      <c r="K78" s="62"/>
+      <c r="L78" s="62"/>
+      <c r="M78" s="62"/>
+      <c r="N78" s="62"/>
+      <c r="O78" s="62"/>
+      <c r="P78" s="62"/>
+      <c r="Q78" s="62"/>
+      <c r="R78" s="62"/>
+      <c r="S78" s="62"/>
+      <c r="T78" s="62"/>
+      <c r="U78" s="62"/>
+      <c r="V78" s="62"/>
+      <c r="W78" s="63"/>
     </row>
     <row r="79" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D79" s="61"/>
@@ -3515,28 +3470,26 @@
       <c r="W83" s="63"/>
     </row>
     <row r="84" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D84" s="58" t="s">
-        <v>39</v>
-      </c>
-      <c r="E84" s="59"/>
-      <c r="F84" s="59"/>
-      <c r="G84" s="59"/>
-      <c r="H84" s="59"/>
-      <c r="I84" s="59"/>
-      <c r="J84" s="59"/>
-      <c r="K84" s="59"/>
-      <c r="L84" s="59"/>
-      <c r="M84" s="59"/>
-      <c r="N84" s="59"/>
-      <c r="O84" s="59"/>
-      <c r="P84" s="59"/>
-      <c r="Q84" s="59"/>
-      <c r="R84" s="59"/>
-      <c r="S84" s="59"/>
-      <c r="T84" s="59"/>
-      <c r="U84" s="59"/>
-      <c r="V84" s="59"/>
-      <c r="W84" s="60"/>
+      <c r="D84" s="61"/>
+      <c r="E84" s="62"/>
+      <c r="F84" s="62"/>
+      <c r="G84" s="62"/>
+      <c r="H84" s="62"/>
+      <c r="I84" s="62"/>
+      <c r="J84" s="62"/>
+      <c r="K84" s="62"/>
+      <c r="L84" s="62"/>
+      <c r="M84" s="62"/>
+      <c r="N84" s="62"/>
+      <c r="O84" s="62"/>
+      <c r="P84" s="62"/>
+      <c r="Q84" s="62"/>
+      <c r="R84" s="62"/>
+      <c r="S84" s="62"/>
+      <c r="T84" s="62"/>
+      <c r="U84" s="62"/>
+      <c r="V84" s="62"/>
+      <c r="W84" s="63"/>
     </row>
     <row r="85" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D85" s="61"/>
@@ -3649,28 +3602,26 @@
       <c r="W89" s="63"/>
     </row>
     <row r="90" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D90" s="58" t="s">
-        <v>40</v>
-      </c>
-      <c r="E90" s="59"/>
-      <c r="F90" s="59"/>
-      <c r="G90" s="59"/>
-      <c r="H90" s="59"/>
-      <c r="I90" s="59"/>
-      <c r="J90" s="59"/>
-      <c r="K90" s="59"/>
-      <c r="L90" s="59"/>
-      <c r="M90" s="59"/>
-      <c r="N90" s="59"/>
-      <c r="O90" s="59"/>
-      <c r="P90" s="59"/>
-      <c r="Q90" s="59"/>
-      <c r="R90" s="59"/>
-      <c r="S90" s="59"/>
-      <c r="T90" s="59"/>
-      <c r="U90" s="59"/>
-      <c r="V90" s="59"/>
-      <c r="W90" s="60"/>
+      <c r="D90" s="61"/>
+      <c r="E90" s="62"/>
+      <c r="F90" s="62"/>
+      <c r="G90" s="62"/>
+      <c r="H90" s="62"/>
+      <c r="I90" s="62"/>
+      <c r="J90" s="62"/>
+      <c r="K90" s="62"/>
+      <c r="L90" s="62"/>
+      <c r="M90" s="62"/>
+      <c r="N90" s="62"/>
+      <c r="O90" s="62"/>
+      <c r="P90" s="62"/>
+      <c r="Q90" s="62"/>
+      <c r="R90" s="62"/>
+      <c r="S90" s="62"/>
+      <c r="T90" s="62"/>
+      <c r="U90" s="62"/>
+      <c r="V90" s="62"/>
+      <c r="W90" s="63"/>
     </row>
     <row r="91" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D91" s="61"/>
@@ -3783,28 +3734,26 @@
       <c r="W95" s="63"/>
     </row>
     <row r="96" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D96" s="58" t="s">
-        <v>41</v>
-      </c>
-      <c r="E96" s="59"/>
-      <c r="F96" s="59"/>
-      <c r="G96" s="59"/>
-      <c r="H96" s="59"/>
-      <c r="I96" s="59"/>
-      <c r="J96" s="59"/>
-      <c r="K96" s="59"/>
-      <c r="L96" s="59"/>
-      <c r="M96" s="59"/>
-      <c r="N96" s="59"/>
-      <c r="O96" s="59"/>
-      <c r="P96" s="59"/>
-      <c r="Q96" s="59"/>
-      <c r="R96" s="59"/>
-      <c r="S96" s="59"/>
-      <c r="T96" s="59"/>
-      <c r="U96" s="59"/>
-      <c r="V96" s="59"/>
-      <c r="W96" s="60"/>
+      <c r="D96" s="61"/>
+      <c r="E96" s="62"/>
+      <c r="F96" s="62"/>
+      <c r="G96" s="62"/>
+      <c r="H96" s="62"/>
+      <c r="I96" s="62"/>
+      <c r="J96" s="62"/>
+      <c r="K96" s="62"/>
+      <c r="L96" s="62"/>
+      <c r="M96" s="62"/>
+      <c r="N96" s="62"/>
+      <c r="O96" s="62"/>
+      <c r="P96" s="62"/>
+      <c r="Q96" s="62"/>
+      <c r="R96" s="62"/>
+      <c r="S96" s="62"/>
+      <c r="T96" s="62"/>
+      <c r="U96" s="62"/>
+      <c r="V96" s="62"/>
+      <c r="W96" s="63"/>
     </row>
     <row r="97" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D97" s="61"/>
@@ -4373,12 +4322,11 @@
       <c r="Z124" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="24">
     <mergeCell ref="R5:W14"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="D36:W36"/>
-    <mergeCell ref="D38:W38"/>
-    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D37:E37"/>
     <mergeCell ref="A123:B124"/>
     <mergeCell ref="Y123:Z124"/>
     <mergeCell ref="C1:X1"/>

</xml_diff>